<commit_message>
Updated Problems to the excel sheet while working with Mux8x1
</commit_message>
<xml_diff>
--- a/Problems_while_designing.xlsx
+++ b/Problems_while_designing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RTL_Desgin_and_Integration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgandhi\OneDrive\RTL_Desgin_and_Integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF1CA1F-491A-4E7F-B666-59B7FF1FB7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA5230A-2D9D-4303-B709-AC461F2BBBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -93,6 +93,35 @@
 correct output.
 s = 0, out = m1
 s= 1, out = m2</t>
+  </si>
+  <si>
+    <t>mux8x1</t>
+  </si>
+  <si>
+    <t>mux8x1.v</t>
+  </si>
+  <si>
+    <t>Warning: "Port size (1) does not match connection size (32) for port i2"</t>
+  </si>
+  <si>
+    <t>While assiging 0 to any variable use e.g. 1'b0 (one bit zero). By default, it will consider 32 bit 0 instead of your required bit zero and it will give you this error.</t>
+  </si>
+  <si>
+    <t>Error (suppressible): (vsim-3053) Illegal output or inout port connection for port 'out'.
+Tried to connect "reg out (8x1) port" to "reg out (4x1) port".</t>
+  </si>
+  <si>
+    <t>port out (8x1) must be defined as wire as it is just driving the out (4x1) port.</t>
+  </si>
+  <si>
+    <t>mux8x1_tb.v</t>
+  </si>
+  <si>
+    <t>GetModuleFileName: The specified module could not be found</t>
+  </si>
+  <si>
+    <t>Need to include mux4x1.v to the tb file.
+Mux4x1 module is instantiated to mux8x1 and included in mux8x1.v file but not to the mux8x1_tb.v. So, by including 4x1 file to tb the error has been resolved.</t>
   </si>
 </sst>
 </file>
@@ -151,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -172,12 +201,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -460,25 +483,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:H39"/>
+  <dimension ref="B5:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="59.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="63.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="59.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="63.88671875" style="2" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
@@ -501,7 +524,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B6" s="5">
         <v>1</v>
       </c>
@@ -513,14 +536,14 @@
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B7" s="5">
         <v>2</v>
       </c>
@@ -534,14 +557,14 @@
         <v>12</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="8" t="s">
+      <c r="H7" s="7" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="6">
         <v>44874</v>
@@ -555,14 +578,14 @@
       <c r="F8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="8" t="s">
+      <c r="H8" s="7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="72" x14ac:dyDescent="0.3">
       <c r="B9" s="5">
         <v>3</v>
       </c>
@@ -578,45 +601,81 @@
       <c r="F9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="8" t="s">
+      <c r="H9" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="5">
         <v>4</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="6">
+        <v>44879</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="6">
+        <v>44879</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B12" s="5">
         <v>5</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="6">
+        <v>44879</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>6</v>
       </c>
@@ -627,7 +686,7 @@
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
@@ -636,7 +695,7 @@
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="5">
         <v>7</v>
       </c>
@@ -647,7 +706,7 @@
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="5">
         <v>8</v>
       </c>
@@ -658,7 +717,7 @@
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
@@ -667,7 +726,7 @@
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="5">
         <v>9</v>
       </c>
@@ -678,7 +737,7 @@
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="5">
         <v>10</v>
       </c>
@@ -689,7 +748,7 @@
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -698,7 +757,7 @@
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="5">
         <v>11</v>
       </c>
@@ -709,7 +768,7 @@
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="5">
         <v>12</v>
       </c>
@@ -720,7 +779,7 @@
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -729,7 +788,7 @@
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -738,7 +797,7 @@
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -747,7 +806,7 @@
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -756,7 +815,7 @@
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -765,7 +824,7 @@
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -774,7 +833,7 @@
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -783,7 +842,7 @@
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -792,7 +851,7 @@
       <c r="G30" s="7"/>
       <c r="H30" s="7"/>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -801,7 +860,7 @@
       <c r="G31" s="7"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -810,7 +869,7 @@
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -819,7 +878,7 @@
       <c r="G33" s="7"/>
       <c r="H33" s="7"/>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -828,7 +887,7 @@
       <c r="G34" s="7"/>
       <c r="H34" s="7"/>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -837,7 +896,7 @@
       <c r="G35" s="7"/>
       <c r="H35" s="7"/>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="5"/>
@@ -846,7 +905,7 @@
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
@@ -855,7 +914,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="5"/>
@@ -864,7 +923,7 @@
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -873,6 +932,218 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
     </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+    </row>
+    <row r="49" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G51" s="7"/>
+      <c r="H51" s="7"/>
+    </row>
+    <row r="52" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G52" s="7"/>
+      <c r="H52" s="7"/>
+    </row>
+    <row r="53" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G53" s="7"/>
+      <c r="H53" s="7"/>
+    </row>
+    <row r="54" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G54" s="7"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G55" s="7"/>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G56" s="7"/>
+      <c r="H56" s="7"/>
+    </row>
+    <row r="57" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G57" s="7"/>
+      <c r="H57" s="7"/>
+    </row>
+    <row r="58" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G58" s="7"/>
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G59" s="7"/>
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G60" s="7"/>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G62" s="7"/>
+      <c r="H62" s="7"/>
+    </row>
+    <row r="63" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G63" s="7"/>
+      <c r="H63" s="7"/>
+    </row>
+    <row r="64" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G64" s="7"/>
+      <c r="H64" s="7"/>
+    </row>
+    <row r="65" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G65" s="7"/>
+      <c r="H65" s="7"/>
+    </row>
+    <row r="66" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G66" s="7"/>
+      <c r="H66" s="7"/>
+    </row>
+    <row r="67" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+    </row>
+    <row r="68" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+    </row>
+    <row r="69" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+    </row>
+    <row r="70" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+    </row>
+    <row r="71" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+    </row>
+    <row r="72" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+    </row>
+    <row r="73" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G73" s="7"/>
+      <c r="H73" s="7"/>
+    </row>
+    <row r="74" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G74" s="7"/>
+      <c r="H74" s="7"/>
+    </row>
+    <row r="75" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G75" s="7"/>
+      <c r="H75" s="7"/>
+    </row>
+    <row r="76" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G76" s="7"/>
+      <c r="H76" s="7"/>
+    </row>
+    <row r="77" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G77" s="7"/>
+      <c r="H77" s="7"/>
+    </row>
+    <row r="78" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G78" s="7"/>
+      <c r="H78" s="7"/>
+    </row>
+    <row r="79" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G79" s="7"/>
+      <c r="H79" s="7"/>
+    </row>
+    <row r="80" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G80" s="7"/>
+      <c r="H80" s="7"/>
+    </row>
+    <row r="81" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+    </row>
+    <row r="82" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G82" s="7"/>
+      <c r="H82" s="7"/>
+    </row>
+    <row r="83" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G83" s="7"/>
+      <c r="H83" s="7"/>
+    </row>
+    <row r="84" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G84" s="7"/>
+      <c r="H84" s="7"/>
+    </row>
+    <row r="85" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G85" s="7"/>
+      <c r="H85" s="7"/>
+    </row>
+    <row r="86" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G86" s="7"/>
+      <c r="H86" s="7"/>
+    </row>
+    <row r="87" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G87" s="7"/>
+      <c r="H87" s="7"/>
+    </row>
+    <row r="88" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G88" s="7"/>
+      <c r="H88" s="7"/>
+    </row>
+    <row r="89" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G89" s="7"/>
+      <c r="H89" s="7"/>
+    </row>
+    <row r="90" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G90" s="7"/>
+      <c r="H90" s="7"/>
+    </row>
+    <row r="91" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G91" s="7"/>
+      <c r="H91" s="7"/>
+    </row>
+    <row r="92" spans="7:8" x14ac:dyDescent="0.3">
+      <c r="G92" s="7"/>
+      <c r="H92" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Problems excel sheet with problems associated with Encoder and Decoder
</commit_message>
<xml_diff>
--- a/Problems_while_designing.xlsx
+++ b/Problems_while_designing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgandhi\OneDrive\RTL_Desgin_and_Integration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA5230A-2D9D-4303-B709-AC461F2BBBCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C35892-3418-4F1F-8E89-7C6E1DF1B015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -122,6 +122,12 @@
   <si>
     <t>Need to include mux4x1.v to the tb file.
 Mux4x1 module is instantiated to mux8x1 and included in mux8x1.v file but not to the mux8x1_tb.v. So, by including 4x1 file to tb the error has been resolved.</t>
+  </si>
+  <si>
+    <t>Primitive output connection must be a scalar net</t>
+  </si>
+  <si>
+    <t>For Gate level implementation : Output of gate should be defined as 'wire' not 'reg'.</t>
   </si>
 </sst>
 </file>
@@ -486,7 +492,7 @@
   <dimension ref="B5:H92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -675,16 +681,28 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13" s="5">
         <v>6</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
+      <c r="C13" s="6">
+        <v>44880</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>

</xml_diff>

<commit_message>
full adder n-bit Implemented n-bit full adder using genvar and parameter overriding concept. Also updated "Problems_while_designing.xlsx" with the problem associated with n-bit full adder.
</commit_message>
<xml_diff>
--- a/Problems_while_designing.xlsx
+++ b/Problems_while_designing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kgandhi\OneDrive\RTL_Desgin_and_Integration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3de0cd961381ec4e/RTL_Design_and_Integration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30C35892-3418-4F1F-8E89-7C6E1DF1B015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{30C35892-3418-4F1F-8E89-7C6E1DF1B015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0BABC4F9-E876-4D87-B6BE-7301E63BAF7A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t>Date</t>
   </si>
@@ -128,6 +128,22 @@
   </si>
   <si>
     <t>For Gate level implementation : Output of gate should be defined as 'wire' not 'reg'.</t>
+  </si>
+  <si>
+    <t>full adder nbit</t>
+  </si>
+  <si>
+    <t>full_adder_nbit.v</t>
+  </si>
+  <si>
+    <t>fa.v</t>
+  </si>
+  <si>
+    <t>Getting expected result but with the delay on one cycle.</t>
+  </si>
+  <si>
+    <t>1 bit full adder was implemented using gates and it required 1 cycle to process 1 bit addition and generate result.
+Replaced gate based 1 bit adder with Data flow model (Using continuous assign) to complete 1 bit addition in single cycle.</t>
   </si>
 </sst>
 </file>
@@ -491,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B5:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -704,14 +720,26 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B14" s="5"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
+      <c r="C14" s="6">
+        <v>44936</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B15" s="5">

</xml_diff>